<commit_message>
Examen y proyecto II bimeste
</commit_message>
<xml_diff>
--- a/03-pandas/data/artwork_data_colores2.xlsx
+++ b/03-pandas/data/artwork_data_colores2.xlsx
@@ -25,12 +25,12 @@
     <t>Paolozzi, Sir Eduardo</t>
   </si>
   <si>
+    <t>Wols</t>
+  </si>
+  <si>
     <t>Jones, Allen</t>
   </si>
   <si>
-    <t>Wols</t>
-  </si>
-  <si>
     <t>Piper, John</t>
   </si>
   <si>
@@ -49,12 +49,12 @@
     <t>Pasmore, Victor</t>
   </si>
   <si>
+    <t>Collins, Cecil</t>
+  </si>
+  <si>
     <t>Tyson, Ian</t>
   </si>
   <si>
-    <t>Collins, Cecil</t>
-  </si>
-  <si>
     <t>Rothenstein, Sir William</t>
   </si>
   <si>
@@ -70,18 +70,18 @@
     <t>Frost, Sir Terry</t>
   </si>
   <si>
+    <t>Palmer, Roger</t>
+  </si>
+  <si>
+    <t>Mordmüller, Rainer G</t>
+  </si>
+  <si>
     <t>Stephenson, Ian</t>
   </si>
   <si>
-    <t>Mordmüller, Rainer G</t>
-  </si>
-  <si>
     <t>Nash, John</t>
   </si>
   <si>
-    <t>Palmer, Roger</t>
-  </si>
-  <si>
     <t>Valoch, Jiri</t>
   </si>
   <si>
@@ -94,181 +94,181 @@
     <t>Vasarely, Victor</t>
   </si>
   <si>
+    <t>Hodgkin, Howard</t>
+  </si>
+  <si>
     <t>Manessier, Alfred</t>
   </si>
   <si>
-    <t>Hodgkin, Howard</t>
+    <t>Salt, John</t>
+  </si>
+  <si>
+    <t>Phillips, Esq Tom</t>
+  </si>
+  <si>
+    <t>Cutts, Simon</t>
+  </si>
+  <si>
+    <t>Art &amp; Language (Michael Baldwin, born 1945; Mel Ramsden, born 1944)</t>
+  </si>
+  <si>
+    <t>Pomodoro, Gio</t>
+  </si>
+  <si>
+    <t>Baselitz, Georg</t>
+  </si>
+  <si>
+    <t>Matisse, Henri</t>
+  </si>
+  <si>
+    <t>Park, Alistair</t>
+  </si>
+  <si>
+    <t>Le Parc, Julio</t>
+  </si>
+  <si>
+    <t>Wentworth, Richard</t>
+  </si>
+  <si>
+    <t>Blake, John</t>
+  </si>
+  <si>
+    <t>Spencer, Sir Stanley</t>
+  </si>
+  <si>
+    <t>Benjamin, Anthony</t>
+  </si>
+  <si>
+    <t>Lindström, Bengt</t>
+  </si>
+  <si>
+    <t>Schneider, Gerard</t>
+  </si>
+  <si>
+    <t>Grayson, Roy</t>
+  </si>
+  <si>
+    <t>Dine, Jim</t>
   </si>
   <si>
     <t>Fabro, Luciano</t>
   </si>
   <si>
+    <t>London Gallery</t>
+  </si>
+  <si>
+    <t>Ackroyd, Norman</t>
+  </si>
+  <si>
+    <t>Baumeister, Willi</t>
+  </si>
+  <si>
+    <t>Stezaker, John</t>
+  </si>
+  <si>
+    <t>Benrath, Frédéric</t>
+  </si>
+  <si>
     <t>Götz, Professor Karl-Otto</t>
   </si>
   <si>
+    <t>King, Ronald</t>
+  </si>
+  <si>
+    <t>Cuixart, Modestos</t>
+  </si>
+  <si>
+    <t>Illes, Arpad</t>
+  </si>
+  <si>
+    <t>Murphy, John</t>
+  </si>
+  <si>
+    <t>Hamilton Finlay, Ian</t>
+  </si>
+  <si>
+    <t>Bird, John</t>
+  </si>
+  <si>
+    <t>Nevinson, Christopher Richard Wynne</t>
+  </si>
+  <si>
+    <t>Braque, Georges</t>
+  </si>
+  <si>
+    <t>Appel, Karel</t>
+  </si>
+  <si>
+    <t>Maccari, Mino</t>
+  </si>
+  <si>
+    <t>Loker, John</t>
+  </si>
+  <si>
+    <t>Neiland, Brendan</t>
+  </si>
+  <si>
+    <t>Disler, Martin</t>
+  </si>
+  <si>
+    <t>Thomkins, André</t>
+  </si>
+  <si>
+    <t>Rocamora, Jaume</t>
+  </si>
+  <si>
+    <t>Rainer, Arnulf</t>
+  </si>
+  <si>
+    <t>Soulages, Pierre</t>
+  </si>
+  <si>
+    <t>Guston, Philip</t>
+  </si>
+  <si>
+    <t>Abrahams, Ivor</t>
+  </si>
+  <si>
+    <t>Downsbrough, Peter</t>
+  </si>
+  <si>
+    <t>Kunkel, Don</t>
+  </si>
+  <si>
+    <t>Hayter, Stanley William</t>
+  </si>
+  <si>
+    <t>Wunderlich, Paul</t>
+  </si>
+  <si>
+    <t>Herring, Ed</t>
+  </si>
+  <si>
+    <t>Blake, Peter</t>
+  </si>
+  <si>
+    <t>Frohner, Adolf</t>
+  </si>
+  <si>
+    <t>Laabs, Hans</t>
+  </si>
+  <si>
+    <t>Sutherland, Graham, OM</t>
+  </si>
+  <si>
     <t>Beuys, Joseph</t>
   </si>
   <si>
-    <t>Soulages, Pierre</t>
-  </si>
-  <si>
-    <t>Loker, John</t>
-  </si>
-  <si>
-    <t>Rocamora, Jaume</t>
-  </si>
-  <si>
-    <t>Spencer, Sir Stanley</t>
-  </si>
-  <si>
-    <t>Baumeister, Willi</t>
-  </si>
-  <si>
-    <t>Baselitz, Georg</t>
-  </si>
-  <si>
-    <t>Park, Alistair</t>
-  </si>
-  <si>
-    <t>Grayson, Roy</t>
-  </si>
-  <si>
-    <t>King, Ronald</t>
-  </si>
-  <si>
-    <t>Nevinson, Christopher Richard Wynne</t>
-  </si>
-  <si>
-    <t>Thomkins, André</t>
-  </si>
-  <si>
-    <t>Neiland, Brendan</t>
+    <t>Irvin, Albert</t>
+  </si>
+  <si>
+    <t>Tamayo, Rufino</t>
+  </si>
+  <si>
+    <t>Lattanzi, Luciano</t>
   </si>
   <si>
     <t>Trevelyan, Julian</t>
-  </si>
-  <si>
-    <t>Murphy, John</t>
-  </si>
-  <si>
-    <t>Ackroyd, Norman</t>
-  </si>
-  <si>
-    <t>Kunkel, Don</t>
-  </si>
-  <si>
-    <t>Irvin, Albert</t>
-  </si>
-  <si>
-    <t>Guston, Philip</t>
-  </si>
-  <si>
-    <t>Stezaker, John</t>
-  </si>
-  <si>
-    <t>Braque, Georges</t>
-  </si>
-  <si>
-    <t>Dine, Jim</t>
-  </si>
-  <si>
-    <t>Art &amp; Language (Michael Baldwin, born 1945; Mel Ramsden, born 1944)</t>
-  </si>
-  <si>
-    <t>Le Parc, Julio</t>
-  </si>
-  <si>
-    <t>Salt, John</t>
-  </si>
-  <si>
-    <t>Wentworth, Richard</t>
-  </si>
-  <si>
-    <t>London Gallery</t>
-  </si>
-  <si>
-    <t>Pomodoro, Gio</t>
-  </si>
-  <si>
-    <t>Hamilton Finlay, Ian</t>
-  </si>
-  <si>
-    <t>Hayter, Stanley William</t>
-  </si>
-  <si>
-    <t>Blake, John</t>
-  </si>
-  <si>
-    <t>Herring, Ed</t>
-  </si>
-  <si>
-    <t>Disler, Martin</t>
-  </si>
-  <si>
-    <t>Cutts, Simon</t>
-  </si>
-  <si>
-    <t>Appel, Karel</t>
-  </si>
-  <si>
-    <t>Downsbrough, Peter</t>
-  </si>
-  <si>
-    <t>Abrahams, Ivor</t>
-  </si>
-  <si>
-    <t>Lindström, Bengt</t>
-  </si>
-  <si>
-    <t>Sutherland, Graham, OM</t>
-  </si>
-  <si>
-    <t>Bird, John</t>
-  </si>
-  <si>
-    <t>Frohner, Adolf</t>
-  </si>
-  <si>
-    <t>Maccari, Mino</t>
-  </si>
-  <si>
-    <t>Benjamin, Anthony</t>
-  </si>
-  <si>
-    <t>Matisse, Henri</t>
-  </si>
-  <si>
-    <t>Laabs, Hans</t>
-  </si>
-  <si>
-    <t>Tamayo, Rufino</t>
-  </si>
-  <si>
-    <t>Phillips, Esq Tom</t>
-  </si>
-  <si>
-    <t>Lattanzi, Luciano</t>
-  </si>
-  <si>
-    <t>Wunderlich, Paul</t>
-  </si>
-  <si>
-    <t>Schneider, Gerard</t>
-  </si>
-  <si>
-    <t>Cuixart, Modestos</t>
-  </si>
-  <si>
-    <t>Rainer, Arnulf</t>
-  </si>
-  <si>
-    <t>Illes, Arpad</t>
-  </si>
-  <si>
-    <t>Blake, Peter</t>
-  </si>
-  <si>
-    <t>Benrath, Frédéric</t>
   </si>
 </sst>
 </file>

</xml_diff>